<commit_message>
Updated models, Model Collection.
</commit_message>
<xml_diff>
--- a/etc/sbml/Chlamydomonas reinhardtii/kegg_ids.xlsx
+++ b/etc/sbml/Chlamydomonas reinhardtii/kegg_ids.xlsx
@@ -7346,8 +7346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1707"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1690" workbookViewId="0">
-      <selection activeCell="E1696" sqref="E1696:E1706"/>
+    <sheetView tabSelected="1" topLeftCell="A1122" workbookViewId="0">
+      <selection activeCell="E1130" sqref="E1130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22871,7 +22871,7 @@
         <v>2289</v>
       </c>
       <c r="E1130" t="s">
-        <v>2289</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="1131" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>